<commit_message>
Ran CompStrDefn pdbs through PolarBearal
</commit_message>
<xml_diff>
--- a/CompStrDefns/DSSP_GT5Final.xlsx
+++ b/CompStrDefns/DSSP_GT5Final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghan/Documents/PhD/GitHubProjects/v6_2018_Network/CompStrDefns/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghan/Documents/PhD/GitProjects/v6_2018_Network/CompStrDefns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F3E1854-D82E-394E-9A66-CEF9DADFFFA9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56FB4D5-B39F-FE43-887D-7017865DE1BB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23260" yWindow="4960" windowWidth="23240" windowHeight="21140" xr2:uid="{0D34EE35-A2AE-6641-97AC-0B098463880C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23240" windowHeight="16560" xr2:uid="{0D34EE35-A2AE-6641-97AC-0B098463880C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
   <si>
     <t>1kmo_A</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>2jmm_A</t>
-  </si>
-  <si>
-    <t>5m2q_A</t>
   </si>
   <si>
     <t>1t16_A</t>
@@ -883,7 +880,7 @@
   <dimension ref="A1:X33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V39" sqref="I39:V39"/>
+      <selection activeCell="K3" sqref="K3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -989,76 +986,70 @@
       <c r="J3">
         <v>0.54961832061068705</v>
       </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3">
-        <v>0.87786259541984701</v>
-      </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
       </c>
       <c r="D4">
         <v>0.113456464379947</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4">
         <v>7.6517150395778305E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4">
         <v>7.6517150395778305E-2</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4">
         <v>9.2348284960422106E-2</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4">
         <v>8.1794195250659604E-2</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N4">
         <v>0.31926121372031602</v>
       </c>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4">
         <v>0.23482849604221601</v>
       </c>
       <c r="Q4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R4">
         <v>0.22163588390501299</v>
       </c>
       <c r="S4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T4">
         <v>0.189973614775725</v>
       </c>
       <c r="U4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V4">
         <v>0.134564643799472</v>
@@ -1066,13 +1057,13 @@
     </row>
     <row r="5" spans="1:24">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
       </c>
       <c r="D5">
         <v>0.117886178861788</v>
@@ -1080,13 +1071,13 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
       </c>
       <c r="D6">
         <v>5.0847457627118599E-2</v>
@@ -1094,73 +1085,73 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
       </c>
       <c r="D7">
         <v>0.133479212253829</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7">
         <v>0.17067833698030599</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7">
         <v>8.97155361050328E-2</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7">
         <v>8.31509846827133E-2</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7">
         <v>8.97155361050328E-2</v>
       </c>
       <c r="M7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N7">
         <v>0.12691466083150901</v>
       </c>
       <c r="O7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P7">
         <v>0.111597374179431</v>
       </c>
       <c r="Q7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R7">
         <v>0.13566739606126901</v>
       </c>
       <c r="S7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T7">
         <v>5.90809628008752E-2</v>
       </c>
       <c r="U7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V7">
         <v>0.129102844638949</v>
       </c>
       <c r="W7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X7">
         <v>0.12035010940919</v>
@@ -1168,13 +1159,13 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
       </c>
       <c r="D8">
         <v>0.110151187904967</v>
@@ -1182,37 +1173,37 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>55</v>
-      </c>
-      <c r="C9" t="s">
-        <v>56</v>
       </c>
       <c r="D9">
         <v>0.15887850467289699</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9">
         <v>5.0467289719626197E-2</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9">
         <v>5.0467289719626197E-2</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J9">
         <v>5.0467289719626197E-2</v>
       </c>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L9">
         <v>5.4205607476635498E-2</v>
@@ -1220,13 +1211,13 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
       </c>
       <c r="D10">
         <v>0.33478260869565202</v>
@@ -1234,13 +1225,13 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>65</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
       </c>
       <c r="D11">
         <v>5.0167224080267497E-2</v>
@@ -1248,25 +1239,25 @@
     </row>
     <row r="12" spans="1:24">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
       </c>
       <c r="D12">
         <v>0.20481927710843301</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12">
         <v>0.19678714859437699</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H12">
         <v>0.19277108433734899</v>
@@ -1274,19 +1265,19 @@
     </row>
     <row r="13" spans="1:24">
       <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
         <v>72</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>73</v>
-      </c>
-      <c r="C13" t="s">
-        <v>74</v>
       </c>
       <c r="D13">
         <v>0.58585858585858497</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F13">
         <v>0.59595959595959602</v>
@@ -1294,13 +1285,13 @@
     </row>
     <row r="14" spans="1:24">
       <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
         <v>76</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>77</v>
-      </c>
-      <c r="C14" t="s">
-        <v>78</v>
       </c>
       <c r="D14">
         <v>8.7452471482889704E-2</v>
@@ -1308,49 +1299,49 @@
     </row>
     <row r="15" spans="1:24">
       <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
         <v>79</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>80</v>
-      </c>
-      <c r="C15" t="s">
-        <v>81</v>
       </c>
       <c r="D15">
         <v>0.16423357664233501</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15">
         <v>0.113138686131386</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15">
         <v>9.4890510948905105E-2</v>
       </c>
       <c r="I15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J15">
         <v>0.37591240875912402</v>
       </c>
       <c r="K15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L15">
         <v>0.14963503649634999</v>
       </c>
       <c r="M15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N15">
         <v>0.36131386861313802</v>
       </c>
       <c r="O15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P15">
         <v>0.42335766423357601</v>
@@ -1358,13 +1349,13 @@
     </row>
     <row r="16" spans="1:24">
       <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
         <v>88</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>89</v>
-      </c>
-      <c r="C16" t="s">
-        <v>90</v>
       </c>
       <c r="D16">
         <v>0.70985915492957696</v>
@@ -1372,61 +1363,61 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
         <v>91</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>92</v>
-      </c>
-      <c r="C17" t="s">
-        <v>93</v>
       </c>
       <c r="D17">
         <v>8.2066869300911893E-2</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F17">
         <v>5.1671732522796297E-2</v>
       </c>
       <c r="G17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H17">
         <v>5.1671732522796297E-2</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J17">
         <v>6.0790273556230998E-2</v>
       </c>
       <c r="K17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L17">
         <v>6.6869300911854002E-2</v>
       </c>
       <c r="M17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N17">
         <v>9.4224924012158096E-2</v>
       </c>
       <c r="O17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P17">
         <v>5.4711246200607799E-2</v>
       </c>
       <c r="Q17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R17">
         <v>5.1671732522796297E-2</v>
       </c>
       <c r="S17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T17">
         <v>5.7750759878419398E-2</v>
@@ -1434,13 +1425,13 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
         <v>102</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>103</v>
-      </c>
-      <c r="C18" t="s">
-        <v>104</v>
       </c>
       <c r="D18">
         <v>0.247311827956989</v>
@@ -1448,19 +1439,19 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
         <v>105</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>106</v>
-      </c>
-      <c r="C19" t="s">
-        <v>107</v>
       </c>
       <c r="D19">
         <v>6.9243156199677899E-2</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19">
         <v>0.19967793880837301</v>
@@ -1468,25 +1459,25 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
         <v>109</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>110</v>
-      </c>
-      <c r="C20" t="s">
-        <v>111</v>
       </c>
       <c r="D20">
         <v>0.16158536585365799</v>
       </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F20">
         <v>9.1463414634146298E-2</v>
       </c>
       <c r="G20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H20">
         <v>0.10060975609756</v>
@@ -1494,25 +1485,25 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" t="s">
         <v>114</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>115</v>
-      </c>
-      <c r="C21" t="s">
-        <v>116</v>
       </c>
       <c r="D21">
         <v>0.56081081081080997</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F21">
         <v>0.59459459459459396</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H21">
         <v>8.1081081081081002E-2</v>
@@ -1520,19 +1511,19 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" t="s">
         <v>119</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>120</v>
-      </c>
-      <c r="C22" t="s">
-        <v>121</v>
       </c>
       <c r="D22">
         <v>0.115384615384615</v>
       </c>
       <c r="E22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F22">
         <v>9.89010989010988E-2</v>
@@ -1540,13 +1531,13 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
         <v>123</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>124</v>
-      </c>
-      <c r="C23" t="s">
-        <v>125</v>
       </c>
       <c r="D23">
         <v>7.6086956521739094E-2</v>
@@ -1554,13 +1545,13 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" t="s">
         <v>126</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>127</v>
-      </c>
-      <c r="C24" t="s">
-        <v>128</v>
       </c>
       <c r="D24">
         <v>0.102920723226703</v>
@@ -1568,13 +1559,13 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" t="s">
         <v>129</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>130</v>
-      </c>
-      <c r="C25" t="s">
-        <v>131</v>
       </c>
       <c r="D25">
         <v>6.1889250814332199E-2</v>
@@ -1582,37 +1573,37 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" t="s">
         <v>132</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>133</v>
-      </c>
-      <c r="C26" t="s">
-        <v>134</v>
       </c>
       <c r="D26">
         <v>7.7830188679245293E-2</v>
       </c>
       <c r="E26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F26">
         <v>9.4339622641509399E-2</v>
       </c>
       <c r="G26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H26">
         <v>5.8962264150943397E-2</v>
       </c>
       <c r="I26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J26">
         <v>7.3113207547169698E-2</v>
       </c>
       <c r="K26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L26">
         <v>0.117924528301886</v>
@@ -1620,43 +1611,43 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" t="s">
         <v>139</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>140</v>
-      </c>
-      <c r="C27" t="s">
-        <v>141</v>
       </c>
       <c r="D27">
         <v>0.36794171220400701</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F27">
         <v>0.36976320582877897</v>
       </c>
       <c r="G27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H27">
         <v>0.21493624772313299</v>
       </c>
       <c r="I27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J27">
         <v>5.1001821493624699E-2</v>
       </c>
       <c r="K27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L27">
         <v>0.21129326047358801</v>
       </c>
       <c r="M27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N27">
         <v>0.10564663023679401</v>
@@ -1664,19 +1655,19 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" t="s">
         <v>147</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>148</v>
-      </c>
-      <c r="C28" t="s">
-        <v>149</v>
       </c>
       <c r="D28">
         <v>0.22902097902097901</v>
       </c>
       <c r="E28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F28">
         <v>0.26223776223776202</v>
@@ -1684,13 +1675,13 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" t="s">
         <v>151</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>152</v>
-      </c>
-      <c r="C29" t="s">
-        <v>153</v>
       </c>
       <c r="D29">
         <v>5.2173913043478203E-2</v>
@@ -1698,13 +1689,13 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" t="s">
         <v>154</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>155</v>
-      </c>
-      <c r="C30" t="s">
-        <v>156</v>
       </c>
       <c r="D30">
         <v>9.9415204678362595E-2</v>
@@ -1712,19 +1703,19 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" t="s">
         <v>157</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>158</v>
-      </c>
-      <c r="C31" t="s">
-        <v>159</v>
       </c>
       <c r="D31">
         <v>5.078125E-2</v>
       </c>
       <c r="E31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F31">
         <v>0.10546875</v>
@@ -1732,13 +1723,13 @@
     </row>
     <row r="32" spans="1:20">
       <c r="A32" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" t="s">
         <v>161</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>162</v>
-      </c>
-      <c r="C32" t="s">
-        <v>163</v>
       </c>
       <c r="D32">
         <v>7.5965130759651195E-2</v>
@@ -1746,19 +1737,19 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" t="s">
         <v>164</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>165</v>
-      </c>
-      <c r="C33" t="s">
-        <v>166</v>
       </c>
       <c r="D33">
         <v>0.10576923076923</v>
       </c>
       <c r="E33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F33">
         <v>7.6923076923076802E-2</v>

</xml_diff>